<commit_message>
Final code with checking and bifurcation and comments
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Матмодели (4 сем)\math-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817FB104-EAD5-4B27-A5EF-2BB8E8916CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CD1F5C-5C22-43A0-874D-2FA197708E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A)" sheetId="1" r:id="rId1"/>
@@ -14740,8 +14740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15905,7 +15905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
@@ -17076,7 +17076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>

</xml_diff>